<commit_message>
resolve error in add student from excel file
</commit_message>
<xml_diff>
--- a/MVC_Attendance/wwwroot/Sheets/newfile.xlsx
+++ b/MVC_Attendance/wwwroot/Sheets/newfile.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Email</t>
   </si>
@@ -36,9 +36,6 @@
     <t>Faculty</t>
   </si>
   <si>
-    <t>zu</t>
-  </si>
-  <si>
     <t>Specialization</t>
   </si>
   <si>
@@ -60,16 +57,34 @@
     <t>UniversityID</t>
   </si>
   <si>
-    <t>kasa@hjjj</t>
-  </si>
-  <si>
     <t>sss</t>
   </si>
   <si>
     <t>as</t>
   </si>
   <si>
-    <t>cairo</t>
+    <t>NumberOfAbsences</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>sssa</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>cgfadg@fgrg</t>
+  </si>
+  <si>
+    <t>fhgsr</t>
+  </si>
+  <si>
+    <t>guygfuy</t>
+  </si>
+  <si>
+    <t>ddd</t>
   </si>
 </sst>
 </file>
@@ -452,10 +467,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -465,69 +480,93 @@
     <col min="4" max="4" width="19.25" customWidth="1"/>
     <col min="5" max="5" width="20.25" customWidth="1"/>
     <col min="7" max="7" width="13.375" customWidth="1"/>
+    <col min="8" max="8" width="13.625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.75" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="7.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="1">
+        <v>123456788</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2">
+        <v>10171077</v>
+      </c>
+      <c r="G2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2">
+        <v>2022</v>
+      </c>
+      <c r="I2">
         <v>0</v>
       </c>
-      <c r="E1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2">
-        <v>123456788</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2">
-        <v>10171077</v>
-      </c>
-      <c r="F2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G2">
-        <v>2020</v>
-      </c>
-      <c r="H2">
+      <c r="J2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2">
         <v>0</v>
       </c>
-      <c r="I2" t="s">
-        <v>13</v>
+      <c r="L2" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="D2" r:id="rId1" display="kasa@hjjj"/>
+    <hyperlink ref="E2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
assign supervisor to tack and intake
</commit_message>
<xml_diff>
--- a/MVC_Attendance/wwwroot/Sheets/newfile.xlsx
+++ b/MVC_Attendance/wwwroot/Sheets/newfile.xlsx
@@ -84,7 +84,7 @@
     <t>guygfuy</t>
   </si>
   <si>
-    <t>ddd</t>
+    <t>dfdgg</t>
   </si>
 </sst>
 </file>
@@ -469,7 +469,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>

</xml_diff>